<commit_message>
feat(catalogo): complete SUNAT Table 22 catalog with all 115 concepts
- Regenerated tabla_ingresos_Plame.xlsx with all 115 official PLAME concepts
  covering codes 0101-0129, 0201-0214, 0301-0314, 0401-0411,
  0501-0507, 0700-0707, 0901-0932
- Updated catalogos_sunat.py hardcoded fallback with the same 115 entries
  (fallback activates when Excel is not found)
- Correct tipo mapping: INGRESO for income/indemnization, DESCUENTO for 07xx
- afecto_afp = OR(SNP, AFP) columns per SUNAT Table 22 specification

fix(login): narrow layout (300px) and high-contrast input text

- Reduced block-container to 300px (was 360px) — more compact and elegant
- Changed input fields to light background (#E8F0FE) with dark text (#0D1B3E)
  fixes white-on-white invisible text issue reported by user
- Added -webkit-text-fill-color and caret-color for cross-browser consistency
- Kept corporate dark card + blue gradient button styling

https://claude.ai/code/session_01F8FhcgyvmhhAUjtZc8xP7W
</commit_message>
<xml_diff>
--- a/tabla_ingresos_Plame.xlsx
+++ b/tabla_ingresos_Plame.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0121</t>
+          <t>0101</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sueldo o Salario Básico</t>
+          <t>ALIMENTACION PRINCIPAL EN DINERO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -488,12 +488,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0122</t>
+          <t>0102</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Salario por hora</t>
+          <t>ALIMENTACION PRINCIPAL EN ESPECIE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -520,12 +520,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>0103</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Asignación Familiar</t>
+          <t>COMISIONES O DESTAJO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -552,12 +552,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0301</t>
+          <t>0104</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bonificación por Producción</t>
+          <t>COMISIONES EVENTUALES A TRABAJADORES</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -584,12 +584,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0302</t>
+          <t>0105</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bonificación por Turno</t>
+          <t>TRABAJO EN SOBRETIEMPO (HORAS EXTRAS) 25%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0303</t>
+          <t>0106</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bonificación por Cumpleaños</t>
+          <t>TRABAJO EN SOBRETIEMPO (HORAS EXTRAS) 35%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,19 +641,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0304</t>
+          <t>0107</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bonificación por Responsabilidad</t>
+          <t>TRABAJO EN DIA FERIADO O DIA DE DESCANSO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -680,12 +680,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0305</t>
+          <t>0108</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bonificación Extraordinaria 9%</t>
+          <t>INCREMENTO EN SNP 3.3%</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -705,19 +705,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0401</t>
+          <t>0109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gratificación Ordinaria Jul/Dic</t>
+          <t>INCREMENTO POR AFILIACION A AFP 10.23%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -737,19 +737,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0110</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gratificación Extraordinaria</t>
+          <t>INCREMENTO POR AFILIACION A AFP 3.00%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -759,29 +759,29 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0601</t>
+          <t>0111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Participación en Utilidades</t>
+          <t>PREMIOS POR VENTAS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -801,19 +801,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0701</t>
+          <t>0112</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Movilidad / Condición de Trabajo</t>
+          <t>PRESTACIONES ALIMENTARIAS - SUMINISTROS DIRECTOS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -823,29 +823,29 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0702</t>
+          <t>0113</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Refrigerio no remunerativo</t>
+          <t>PRESTACIONES ALIMENTARIAS - SUMINISTROS INDIRECTOS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -872,12 +872,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0801</t>
+          <t>0114</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Horas Extras 25%</t>
+          <t>VACACIONES TRUNCAS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -904,12 +904,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0802</t>
+          <t>0115</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Horas Extras 35%</t>
+          <t>REMUNERACION DIA DE DESCANSO Y FERIADOS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -936,12 +936,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0901</t>
+          <t>0116</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Comisiones</t>
+          <t>REMUNERACION EN ESPECIE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -968,12 +968,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0903</t>
+          <t>0117</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Otros Ingresos Gravados</t>
+          <t>COMPENSACION VACACIONAL</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1000,96 +1000,3136 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0904</t>
+          <t>0118</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Adelanto de Remuneraciones</t>
+          <t>REMUNERACION VACACIONAL</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>DESCUENTO</t>
+          <t>INGRESO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0905</t>
+          <t>0119</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Descuento Judicial Alimentos</t>
+          <t>REMUNERACIONES DEVENGADAS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>DESCUENTO</t>
+          <t>INGRESO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>0120</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUBVENCION ECONOMICA MENSUAL (PRACTICANTE SENATI)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0121</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>REMUNERACION O JORNAL BASICO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0122</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>REMUNERACION PERMANENTE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0123</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>REMUNERACION DE LOS SOCIOS DE COOPERATIVAS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0124</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>REMUNERACION POR LA HORA DE PERMISO POR LACTANCIA</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0125</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>REMUNERACION INTEGRAL ANUAL - CUOTA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0126</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>INGRESOS DEL CONDUCTOR DE LA MICROEMPRESA AFILIADO AL SIS</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0127</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>INGRESOS DEL CONDUCTOR DE LA MICROEMPRESA - SEGURO REGULAR</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0128</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>REMUNERACION QUE EXCEDE EL VALOR DE MERCADO (DIVIDENDOS)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0129</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ESTIPENDIO MENSUAL INTERNO CIENCIAS DE LA SALUD</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0201</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ASIGNACION FAMILIAR</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0202</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ASIGNACION O BONIFICACION POR EDUCACION</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0203</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR CUMPLEANOS</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>0204</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR MATRIMONIO</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0205</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR NACIMIENTO DE HIJOS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0206</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR FALLECIMIENTO DE FAMILIARES</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0207</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR OTROS MOTIVOS PERSONALES</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0208</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR FESTIVIDAD</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0209</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ASIGNACION PROVISIONAL POR DEMANDA DE TRABAJADOR DESPEDIDO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0210</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ASIGNACION VACACIONAL</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>0211</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR ESCOLARIDAD 30 JORNALES BASICOS/ANO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0212</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ASIGNACIONES OTORGADAS POR UNICA VEZ CON MOTIVO DE CIERTAS CONTINGENCIAS</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>0213</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ASIGNACIONES OTORGADAS REGULARMENTE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>0214</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ASIGNACION POR FALLECIMIENTO 1 UIT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0301</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BONIFICACION POR 25 Y 30 ANOS DE SERVICIOS</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0302</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BONIFICACION POR CIERRE DE PLIEGO</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0303</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>BONIFICACION POR PRODUCCION, ALTURA, TURNO, ETC.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>0304</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BONIFICACION POR RIESGO DE CAJA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>0305</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BONIFICACIONES POR TIEMPO DE SERVICIOS</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>0306</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BONIFICACIONES REGULARES</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>0307</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BONIFICACIONES CAFAE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>0308</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>COMPENSACION POR TRABAJOS EN DIAS DE DESCANSO Y EN FERIADOS</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>0309</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>BONIFICACION POR TURNO NOCTURNO 20% JORNAL BASICO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>0310</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BONIFICACION CONTACTO DIRECTO CON AGUA 20% JORNAL BASICO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>0311</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>BONIFICACION UNIFICADA DE CONSTRUCCION</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>0312</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>BONIFICACION EXTRAORDINARIA TEMPORAL - LEY 29351 Y 30334</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>0313</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>BONIFICACION EXTRAORDINARIA PROPORCIONAL - LEY 29351 Y 30334</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>0314</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BONIFICACION ESPECIAL POR TRABAJO AGRARIO LEY 31110 - BETA</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>0401</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES DE FIESTAS PATRIAS Y NAVIDAD</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>0402</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>OTRAS GRATIFICACIONES ORDINARIAS</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>0403</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES EXTRAORDINARIAS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>0404</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>AGUINALDOS DE JULIO Y DICIEMBRE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>0405</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES PROPORCIONAL</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>0406</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES DE FIESTAS PATRIAS Y NAVIDAD - LEY 29351 Y 30334</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>0407</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES PROPORCIONAL - LEY 29351 Y 30334</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>0408</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>GRATIFIC FIESTAS PATRIAS Y NAVIDAD TRABAJ PESQ LEY 30334</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>0409</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>GRATIFICACIONES PROPORCIONAL/TRUNCA TRABAJ PESQUEROS LEY 30334</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>0410</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>GRATIF FORMA PARTE REMUNER EXCEDE VALOR DE MERCADO (DIVIDENDO)</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>0411</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>GRATIF PAGADAS INTERNOS SALUD DU 090-2020 Y OTROS NO GRAVADOS ESSALUD</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>0501</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR DESPIDO INJUSTIFICADO U HOSTILIDAD</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>0502</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR MUERTE O INCAPACIDAD</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>0503</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR RESOLUCION DE CONTRATO SUJETO A MODALIDAD</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>0504</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR VACACIONES NO GOZADAS</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>0505</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR RETENCION INDEBIDA DE CTS ART. 52 DS 001-97-TR</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>0506</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR NO REINCORPORAR A UN TRABAJADOR CESADO EN CESE COLECTIVO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>0507</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>INDEMNIZACION POR REALIZAR HORAS EXTRAS IMPUESTAS POR EL EMPLEADOR</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>0700</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DESCUENTOS AL TRABAJADOR</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>0701</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ADELANTO SUELDO</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>0702</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CUOTA SINDICAL</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>0703</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DESCUENTO AUTORIZADO U ORDENADO POR MANDATO JUDICIAL</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>0704</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>TARDANZAS</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>0705</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>INASISTENCIAS</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>0706</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>OTROS DESCUENTOS NO DEDUCIBLES DE LA BASE IMPONIBLE</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>0707</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>OTROS DESCUENTOS DEDUCIBLES DE LA BASE IMPONIBLE</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>DESCUENTO</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>0901</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>BIENES DE LA PROPIA EMPRESA OTORGADOS PARA EL CONSUMO DEL TRABAJADOR</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>0902</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>BONO DE PRODUCTIVIDAD</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>0903</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CANASTA DE NAVIDAD O SIMILARES</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>0904</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>COMPENSACION POR TIEMPO DE SERVICIOS</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>0905</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>GASTOS DE REPRESENTACION - LIBRE DISPONIBILIDAD</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
           <t>0906</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Prestamo del Empleador</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>DESCUENTO</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>N</t>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>INCENTIVO POR CESE DEL TRABAJADOR</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>0907</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LICENCIA CON GOCE DE HABER</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>0908</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MOVILIDAD DE LIBRE DISPOSICION</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>0909</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>MOVILIDAD SUPEDITADA A ASISTENCIA Y QUE CUBRE SOLO EL TRASLADO</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>0910</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>PARTICIPACION EN LAS UTILIDADES - PAGADAS ANTES DE LA DECLARACION ANUAL IR</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>0911</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PARTICIPACION EN LAS UTILIDADES - PAGADAS DESPUES DE LA DECLARACION ANUAL IR</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>0912</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PENSIONES DE JUBILACION O CESANTIA, MONTEPIO O INVALIDEZ</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>0913</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>RECARGO AL CONSUMO</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>0914</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>REFRIGERIO QUE NO ES ALIMENTACION PRINCIPAL</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>0915</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>SUBSIDIOS POR MATERNIDAD</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>0916</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>SUBSIDIOS DE INCAPACIDAD POR ENFERMEDAD</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>0917</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>CONDICIONES DE TRABAJO</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>0918</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>IMPUESTO A LA RENTA DE QUINTA CATEGORIA ASUMIDO</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>0919</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SISTEMA NACIONAL DE PENSIONES ASUMIDO</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>0920</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SISTEMA PRIVADO DE PENSIONES ASUMIDO</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>0921</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>PENSIONES DE JUBILACION PENDIENTES POR LIQUIDAR</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>0922</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>SUMAS O BIENES QUE NO SON DE LIBRE DISPOSICION</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>0923</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>INGRESOS DE CUARTA CATEGORIA CONSIDERADOS DE QUINTA CATEGORIA</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>0924</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>INGRESOS CUARTA-QUINTA SIN RELACION DE DEPENDENCIA</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>0925</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>INGRESO DEL PESCADOR ARTESANAL INDEPENDIENTE - BASE APORTE ESSALUD</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>0926</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>TRANSFERENCIA DIRECTA AL EXPESCADOR - LEY 30003</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>0927</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>BONIFICACION PRIMA TEXTIL</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>0928</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>DEVOLUCION RETENCION EXCESO IMP. RENTA 5TA CAT.</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>0929</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>OTRAS ASIGNACIONES QUE EXCEDEN VALOR DE MERCADO (DIVIDENDOS)</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>0930</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>REMUNERACION QUE EXCEDE VALOR DE MERCADO DE PERIODOS ANTERIORES</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>0931</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>PARTICIPACION PESCA CAPTURADA</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>0932</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>REMUNERACION TRAB PESQUEROS GRAVADA CON REP ARM Y REP TRAB</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>INGRESO</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>S</t>
         </is>
       </c>
     </row>

</xml_diff>